<commit_message>
update metadata description for chc20
</commit_message>
<xml_diff>
--- a/codebook/bio_metadata_archive.xlsx
+++ b/codebook/bio_metadata_archive.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoregon-my.sharepoint.com/personal/strevino_uoregon_edu/Documents/Desktop/Maria's Research/Turning Points 4 Women/TurningPoints4Women-GitHubRepo/do_not_push/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoregon-my.sharepoint.com/personal/strevino_uoregon_edu/Documents/Desktop/Maria's Research/Turning Points 4 Women/TurningPoints4Women-GitHubRepo/codebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{4129E356-5065-4A27-A81F-61F34F4782D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7599E8E-719A-422E-A94F-1EA563FBD088}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{4129E356-5065-4A27-A81F-61F34F4782D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93A563E0-87CD-4CA3-AD22-845236C49FB1}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-12" windowWidth="23256" windowHeight="12576" xr2:uid="{DDDA4171-1007-4242-96C4-7294A1D02362}"/>
   </bookViews>
@@ -1200,9 +1200,6 @@
     <t>19e. Is it ongoing?</t>
   </si>
   <si>
-    <t>20a. Any other conditions? - Selected Choice</t>
-  </si>
-  <si>
     <t>20c. Were you diagnosed with this condition?</t>
   </si>
   <si>
@@ -1258,6 +1255,9 @@
   </si>
   <si>
     <t>Minutes since last time participant ate anything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20a. Any other conditions? </t>
   </si>
 </sst>
 </file>
@@ -1656,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCE9083-857B-4810-BFFA-6D0B4550C4AB}">
   <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,7 +1735,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1743,7 +1743,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1791,7 +1791,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1799,7 +1799,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1831,7 +1831,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1903,7 +1903,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1911,7 +1911,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1935,7 +1935,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1951,15 +1951,15 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B37" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -3255,7 +3255,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>378</v>
+        <v>397</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -3263,7 +3263,7 @@
         <v>198</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -3271,7 +3271,7 @@
         <v>199</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3279,7 +3279,7 @@
         <v>200</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>